<commit_message>
add better search engine
</commit_message>
<xml_diff>
--- a/Service/Reports/ShopToolsList.xlsx
+++ b/Service/Reports/ShopToolsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\FinishedShopApp\venv\TempSource\Service\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{33F25824-F245-4689-BD1A-D7BF938C511F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1851D16C-7D4C-4A38-BF5A-A2949FF46D05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CEA7B18F-0EDF-4F76-84FF-B52E9CA7BF6C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Starrett-Calipers</t>
+  </si>
+  <si>
+    <t>Standard-Wrench_open-end</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9CD742-3893-45E5-AF71-D17E57EE27A3}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +545,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A26" si="0">A3+1</f>
+        <f t="shared" ref="A4:A37" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -820,6 +823,99 @@
       </c>
       <c r="C26" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>